<commit_message>
graphs for 2108 mb
</commit_message>
<xml_diff>
--- a/projeto1/test/graphs/xls/aprox-error-1-2108MB.xlsx
+++ b/projeto1/test/graphs/xls/aprox-error-1-2108MB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\betoc\Documents\git\string-processing\projeto1\test\graphs\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cavalcanti/Documents/git/ufpe/string-processing/projeto1/test/graphs/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB6CED3-C0F9-6247-8B68-9F3769A9F556}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="result-aprox-error-1-50MB" sheetId="1" r:id="rId1"/>
@@ -108,7 +109,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -619,10 +620,10 @@
     <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorreto" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutra" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Ruim" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -680,18 +681,13 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR"/>
-              <a:t>Resultado Aproximad</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="pt-BR" baseline="0"/>
-              <a:t>o english.2108MB - Erro: 1</a:t>
+              <a:t>Arquivo 2108MB - Busca Aproximada - Erro: 1</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -913,8 +909,223 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'result-aprox-error-1-50MB'!$A$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wu-manber</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="24"/>
+              <c:pt idx="0">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>11</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>12</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>13</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>14</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>15</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>16</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>17</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>18</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>19</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>21</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>22</c:v>
+              </c:pt>
+              <c:pt idx="21">
+                <c:v>23</c:v>
+              </c:pt>
+              <c:pt idx="22">
+                <c:v>24</c:v>
+              </c:pt>
+              <c:pt idx="23">
+                <c:v>25</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'result-aprox-error-1-50MB'!$E$41:$E$65</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'result-aprox-error-1-50MB'!$E$42:$E$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>22.43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.678999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.507</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.816000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.573</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.034000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.411</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.885999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.605</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.505000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.853</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.771000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.407999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.61</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14.031000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.789</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14.481</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.635999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14.522</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15.606999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14.186999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15.459</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>15.488</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-B87A-43C1-826D-E90174DD1A5D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>'result-aprox-error-1-50MB'!$A$34</c:f>
@@ -1124,221 +1335,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000012-B87A-43C1-826D-E90174DD1A5D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'result-aprox-error-1-50MB'!$A$45</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>wu-manber</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="24"/>
-              <c:pt idx="0">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>3</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>4</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>5</c:v>
-              </c:pt>
-              <c:pt idx="4">
-                <c:v>6</c:v>
-              </c:pt>
-              <c:pt idx="5">
-                <c:v>7</c:v>
-              </c:pt>
-              <c:pt idx="6">
-                <c:v>8</c:v>
-              </c:pt>
-              <c:pt idx="7">
-                <c:v>9</c:v>
-              </c:pt>
-              <c:pt idx="8">
-                <c:v>10</c:v>
-              </c:pt>
-              <c:pt idx="9">
-                <c:v>11</c:v>
-              </c:pt>
-              <c:pt idx="10">
-                <c:v>12</c:v>
-              </c:pt>
-              <c:pt idx="11">
-                <c:v>13</c:v>
-              </c:pt>
-              <c:pt idx="12">
-                <c:v>14</c:v>
-              </c:pt>
-              <c:pt idx="13">
-                <c:v>15</c:v>
-              </c:pt>
-              <c:pt idx="14">
-                <c:v>16</c:v>
-              </c:pt>
-              <c:pt idx="15">
-                <c:v>17</c:v>
-              </c:pt>
-              <c:pt idx="16">
-                <c:v>18</c:v>
-              </c:pt>
-              <c:pt idx="17">
-                <c:v>19</c:v>
-              </c:pt>
-              <c:pt idx="18">
-                <c:v>20</c:v>
-              </c:pt>
-              <c:pt idx="19">
-                <c:v>21</c:v>
-              </c:pt>
-              <c:pt idx="20">
-                <c:v>22</c:v>
-              </c:pt>
-              <c:pt idx="21">
-                <c:v>23</c:v>
-              </c:pt>
-              <c:pt idx="22">
-                <c:v>24</c:v>
-              </c:pt>
-              <c:pt idx="23">
-                <c:v>25</c:v>
-              </c:pt>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:autoCat val="1"/>
-                </c:ext>
-              </c:extLst>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'result-aprox-error-1-50MB'!$E$41:$E$65</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'result-aprox-error-1-50MB'!$E$42:$E$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>22.43</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18.678999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14.54</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.507</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15.816000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14.573</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14.034000000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14.411</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>13.885999999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14.605</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>14.505000000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13.853</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13.771000000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14.407999999999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14.61</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>14.031000000000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>14.789</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>14.481</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>14.635999999999999</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>14.522</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>15.606999999999999</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>14.186999999999999</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>15.459</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>15.488</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000013-B87A-43C1-826D-E90174DD1A5D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1393,7 +1389,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1493,7 +1488,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -1516,7 +1511,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1526,7 +1520,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -1591,7 +1585,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2218,7 +2211,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2498,19 +2497,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F65"/>
+    <sheetView tabSelected="1" topLeftCell="G11" workbookViewId="0">
+      <selection activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2530,7 +2529,7 @@
         <v>85693257</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2550,7 +2549,7 @@
         <v>52005942</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2570,7 +2569,7 @@
         <v>2617922</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2590,7 +2589,7 @@
         <v>1047906</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2610,7 +2609,7 @@
         <v>534633</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2630,7 +2629,7 @@
         <v>107108</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -2650,7 +2649,7 @@
         <v>100677</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2670,7 +2669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2690,7 +2689,7 @@
         <v>140151</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -2710,7 +2709,7 @@
         <v>2471</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -2730,7 +2729,7 @@
         <v>4289</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -2750,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -2770,7 +2769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -2790,7 +2789,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2810,7 +2809,7 @@
         <v>35165576</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2830,7 +2829,7 @@
         <v>31558755</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2850,7 +2849,7 @@
         <v>2576332</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2870,7 +2869,7 @@
         <v>1034752</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -2890,7 +2889,7 @@
         <v>531619</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -2910,7 +2909,7 @@
         <v>106934</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -2930,7 +2929,7 @@
         <v>100595</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -2950,7 +2949,7 @@
         <v>30209</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -2970,7 +2969,7 @@
         <v>139741</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -2990,7 +2989,7 @@
         <v>2467</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -3010,7 +3009,7 @@
         <v>4266</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -3030,7 +3029,7 @@
         <v>26722</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -3050,7 +3049,7 @@
         <v>4122</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -3070,7 +3069,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -3090,7 +3089,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -3110,7 +3109,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -3130,7 +3129,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -3150,7 +3149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -3170,7 +3169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -3190,7 +3189,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -3210,7 +3209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -3230,7 +3229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -3250,7 +3249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -3270,7 +3269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -3290,7 +3289,7 @@
         <v>35170328</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -3310,7 +3309,7 @@
         <v>31570373</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -3330,7 +3329,7 @@
         <v>2584194</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -3350,7 +3349,7 @@
         <v>1036657</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -3370,7 +3369,7 @@
         <v>532138</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -3390,7 +3389,7 @@
         <v>107141</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -3410,7 +3409,7 @@
         <v>100732</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>26</v>
       </c>
@@ -3430,7 +3429,7 @@
         <v>30297</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -3450,7 +3449,7 @@
         <v>139797</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -3470,7 +3469,7 @@
         <v>2508</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>26</v>
       </c>
@@ -3490,7 +3489,7 @@
         <v>4292</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -3510,7 +3509,7 @@
         <v>26739</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -3530,7 +3529,7 @@
         <v>4127</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>26</v>
       </c>
@@ -3550,7 +3549,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -3570,7 +3569,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>26</v>
       </c>
@@ -3590,7 +3589,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>26</v>
       </c>
@@ -3610,7 +3609,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -3630,7 +3629,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -3650,7 +3649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -3670,7 +3669,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -3690,7 +3689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -3710,7 +3709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -3730,7 +3729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>26</v>
       </c>

</xml_diff>